<commit_message>
add envelopes to the loadcase generation script
</commit_message>
<xml_diff>
--- a/11 Loadcases.xlsx
+++ b/11 Loadcases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rob\repos\LusasNoteBooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906E9B2A-A164-4825-B519-72F14AE2380F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0027CD0-63D1-46F3-8C5D-7D4FF85B5DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1620" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Loadcases" sheetId="1" r:id="rId1"/>
+    <sheet name="Envelopes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Self Weight</t>
   </si>
@@ -64,13 +65,82 @@
   </si>
   <si>
     <t>Moving Load Characteristic</t>
+  </si>
+  <si>
+    <t>Loadcases</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>FindSimilar</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Traffic 1</t>
+  </si>
+  <si>
+    <t>Traffic 2</t>
+  </si>
+  <si>
+    <t>Traffic 3</t>
+  </si>
+  <si>
+    <t>Traffic 4</t>
+  </si>
+  <si>
+    <t>Traffic 5</t>
+  </si>
+  <si>
+    <t>Traffic 6</t>
+  </si>
+  <si>
+    <t>Traffic 7</t>
+  </si>
+  <si>
+    <t>Traffic 8</t>
+  </si>
+  <si>
+    <t>Traffic 9</t>
+  </si>
+  <si>
+    <t>Traffic 10</t>
+  </si>
+  <si>
+    <t>Name = Name of envelope to be created</t>
+  </si>
+  <si>
+    <t>Loadcases = Name of loadcases to be included in the envelope</t>
+  </si>
+  <si>
+    <t>FindSimilar = Use all loadsets that start with the loadcase name</t>
+  </si>
+  <si>
+    <t>Name = Name of loadcase to be created</t>
+  </si>
+  <si>
+    <t>Count = Number of similar loadcases to be created = default empty = 1</t>
+  </si>
+  <si>
+    <t>Analysis = Name of the analysis in which to create the loadcase</t>
+  </si>
+  <si>
+    <t>Prestress</t>
+  </si>
+  <si>
+    <t>Gravity</t>
+  </si>
+  <si>
+    <t>Gravity = Automatically apply gravity to the loadcase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +152,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,9 +190,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -392,19 +479,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -412,71 +500,255 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803832CE-E52E-47CE-865F-4A6C7DB9A262}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>